<commit_message>
feat(schedule): add pending fixes and exclude invalid postcodes
</commit_message>
<xml_diff>
--- a/testFiles/P3 test.xlsx
+++ b/testFiles/P3 test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6718527680502480/Coding/ICjourney/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{6C0AF0A5-A6DE-44D5-BB54-F51C7CD1DE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{078339A0-EAA1-428C-8437-14960CB30753}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{6C0AF0A5-A6DE-44D5-BB54-F51C7CD1DE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EAD496B-CB53-4AED-BC8F-995E9C8BA1AF}"/>
   <bookViews>
-    <workbookView xWindow="32145" yWindow="-1950" windowWidth="27390" windowHeight="19200" xr2:uid="{E38F686A-5AAA-4C21-B0FD-6A5596417B7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E38F686A-5AAA-4C21-B0FD-6A5596417B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
     <t>Kessingland Utd WMC(Kessingland)ECI</t>
   </si>
   <si>
-    <t>NR33 7QD</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
   </si>
   <si>
     <t>Quayside Bar &amp; Restaurant (the waterfront probs)</t>
-  </si>
-  <si>
-    <t>NR33 9JY</t>
   </si>
   <si>
     <t>Rob Brown (adam moss and co probs)</t>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t>Rob Brown (kirsty smith account manager)</t>
+  </si>
+  <si>
+    <t>nr33</t>
+  </si>
+  <si>
+    <t>nr</t>
   </si>
 </sst>
 </file>
@@ -25477,6 +25477,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25799,7 +25803,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:L16"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26029,7 +26033,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>19</v>
@@ -26038,7 +26042,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="12" t="str">
         <f>IFERROR(VLOOKUP(B6, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26071,10 +26075,10 @@
     </row>
     <row r="7" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>19</v>
@@ -26083,7 +26087,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="12" t="str">
         <f>IFERROR(VLOOKUP(B7, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26116,10 +26120,10 @@
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>19</v>
@@ -26161,10 +26165,10 @@
     </row>
     <row r="9" spans="1:12" ht="81" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>19</v>
@@ -26173,7 +26177,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" s="12" t="str">
         <f>IFERROR(VLOOKUP(B9, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26206,10 +26210,10 @@
     </row>
     <row r="10" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>19</v>
@@ -26251,10 +26255,10 @@
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>19</v>
@@ -26296,10 +26300,10 @@
     </row>
     <row r="12" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>19</v>
@@ -26308,7 +26312,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="12" t="str">
         <f>IFERROR(VLOOKUP(B12, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26341,10 +26345,10 @@
     </row>
     <row r="13" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>19</v>
@@ -26353,7 +26357,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F13" s="12" t="str">
         <f>IFERROR(VLOOKUP(B13, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26386,10 +26390,10 @@
     </row>
     <row r="14" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>19</v>
@@ -26431,10 +26435,10 @@
     </row>
     <row r="15" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>19</v>
@@ -26476,10 +26480,10 @@
     </row>
     <row r="16" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>19</v>
@@ -26488,7 +26492,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F16" s="12" t="str">
         <f>IFERROR(VLOOKUP(B16, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>

</xml_diff>